<commit_message>
added script for end to end testing
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh Kumar Samal\PycharmProjects\orangeHrm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\batch10\batch10\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7234C9F-EFC7-460E-8D36-315F1DF1A00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F9C066-8F43-40EA-8152-74B4C4D1F0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5364" yWindow="1032" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
+    <sheet name="testdata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -43,6 +44,21 @@
   </si>
   <si>
     <t>admin7896</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>pintu</t>
+  </si>
+  <si>
+    <t>samal</t>
   </si>
 </sst>
 </file>
@@ -362,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -407,4 +423,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AAB44F-DBE5-4F58-AD57-19E8F7F4DAF4}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>755004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>